<commit_message>
Update Patenting option valuation.xlsx
</commit_message>
<xml_diff>
--- a/Patenting option valuation.xlsx
+++ b/Patenting option valuation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8C04ED-1B80-466E-A5ED-713778AE0EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0301E05-3447-4020-9053-F6D756FC9925}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{400703B4-251B-49D8-B8CB-49BA2528FB4C}"/>
+    <workbookView xWindow="2040" yWindow="-110" windowWidth="36470" windowHeight="21820" activeTab="1" xr2:uid="{400703B4-251B-49D8-B8CB-49BA2528FB4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Valuation" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Royalty Rate</t>
   </si>
@@ -340,23 +340,6 @@
   </si>
   <si>
     <t>R</t>
-  </si>
-  <si>
-    <r>
-      <t>V</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>P</t>
-    </r>
   </si>
   <si>
     <t>Marginal company valuation per patent portfolio asset</t>
@@ -479,6 +462,25 @@
   <si>
     <t>Probability of future market adoption</t>
   </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>P</t>
+    </r>
+  </si>
+  <si>
+    <t>Directions: Enter estimates in the colored boxes below to compute the net present value at the bottom line</t>
+  </si>
 </sst>
 </file>
 
@@ -487,9 +489,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[&gt;=1000000000]&quot;$&quot;#,##0,,,&quot; B&quot;;[&gt;=1000000]&quot;$&quot;#0,,&quot; M&quot;;&quot;$&quot;#0,&quot; K&quot;"/>
     <numFmt numFmtId="165" formatCode="[=1]#;[=0]&quot;&quot;;#.###"/>
-    <numFmt numFmtId="167" formatCode="[&gt;=1000000000]&quot;$&quot;#,##0.0,,,&quot; B&quot;;[&gt;=1000000]\ &quot;$&quot;#0.0,,&quot; M&quot;;\ &quot;$&quot;#0.0,&quot; K&quot;"/>
+    <numFmt numFmtId="166" formatCode="[&gt;=1000000000]&quot;$&quot;#,##0.0,,,&quot; B&quot;;[&gt;=1000000]\ &quot;$&quot;#0.0,,&quot; M&quot;;\ &quot;$&quot;#0.0,&quot; K&quot;"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,13 +574,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -590,8 +585,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
@@ -599,18 +592,10 @@
     </font>
     <font>
       <b/>
-      <i/>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -843,16 +828,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="dashed">
         <color auto="1"/>
       </left>
-      <right style="double">
+      <right style="dashed">
         <color auto="1"/>
       </right>
-      <top style="double">
+      <top style="dashed">
         <color auto="1"/>
       </top>
-      <bottom style="double">
+      <bottom style="dashed">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -861,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -898,7 +883,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -952,29 +936,8 @@
     <xf numFmtId="164" fontId="10" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -985,30 +948,49 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="11" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="11" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="11" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="4" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="15" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1350,7 +1332,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Accurate Valuation'!$F$13:$F$32</c:f>
+              <c:f>'Accurate Valuation'!$F$9:$F$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1438,7 +1420,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Accurate Valuation'!$H$13:$H$32</c:f>
+              <c:f>'Accurate Valuation'!$H$9:$H$28</c:f>
               <c:numCache>
                 <c:formatCode>[&gt;=1000000000]"$"#,##0,,," B";[&gt;=1000000]"$"#0,," M";"$"#0," K"</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1526,7 +1508,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Accurate Valuation'!$I$13:$I$32</c:f>
+              <c:f>'Accurate Valuation'!$I$9:$I$28</c:f>
               <c:numCache>
                 <c:formatCode>[&gt;=1000000000]"$"#,##0,,," B";[&gt;=1000000]"$"#0,," M";"$"#0," K"</c:formatCode>
                 <c:ptCount val="20"/>
@@ -2316,19 +2298,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>374650</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 2">
@@ -2342,8 +2324,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1397000" y="450850"/>
-              <a:ext cx="10464800" cy="1035050"/>
+              <a:off x="8483600" y="7150100"/>
+              <a:ext cx="6781800" cy="787400"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2479,7 +2461,7 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -2492,7 +2474,7 @@
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -2506,7 +2488,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -2520,7 +2502,7 @@
                       </m:sub>
                     </m:sSub>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                         <a:solidFill>
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
@@ -2534,7 +2516,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -2549,7 +2531,7 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                              <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                 <a:solidFill>
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
@@ -2565,7 +2547,7 @@
                               <m:naryPr>
                                 <m:chr m:val="∑"/>
                                 <m:ctrlPr>
-                                  <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                  <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                     <a:solidFill>
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
@@ -2578,7 +2560,7 @@
                               </m:naryPr>
                               <m:sub>
                                 <m:r>
-                                  <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                                  <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                                     <a:solidFill>
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
@@ -2590,7 +2572,7 @@
                                   <m:t>𝑖</m:t>
                                 </m:r>
                                 <m:r>
-                                  <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                                  <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                                     <a:solidFill>
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
@@ -2604,7 +2586,7 @@
                                 <m:sSub>
                                   <m:sSubPr>
                                     <m:ctrlPr>
-                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -2617,7 +2599,7 @@
                                   </m:sSubPr>
                                   <m:e>
                                     <m:r>
-                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -2631,7 +2613,7 @@
                                   </m:e>
                                   <m:sub>
                                     <m:r>
-                                      <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -2647,7 +2629,7 @@
                               </m:sub>
                               <m:sup>
                                 <m:r>
-                                  <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                  <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                     <a:solidFill>
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
@@ -2659,7 +2641,7 @@
                                   <m:t>2</m:t>
                                 </m:r>
                                 <m:r>
-                                  <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                                  <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                                     <a:solidFill>
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
@@ -2675,7 +2657,7 @@
                                 <m:f>
                                   <m:fPr>
                                     <m:ctrlPr>
-                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -2690,7 +2672,7 @@
                                     <m:sSub>
                                       <m:sSubPr>
                                         <m:ctrlPr>
-                                          <a:rPr lang="en-US" sz="1800" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1400" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -2703,7 +2685,7 @@
                                       </m:sSubPr>
                                       <m:e>
                                         <m:r>
-                                          <a:rPr lang="en-US" sz="1800" b="0" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1400" b="0" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -2717,7 +2699,7 @@
                                       </m:e>
                                       <m:sub>
                                         <m:r>
-                                          <a:rPr lang="en-US" sz="1800" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1400" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -2731,7 +2713,7 @@
                                       </m:sub>
                                     </m:sSub>
                                     <m:r>
-                                      <a:rPr lang="en-US" sz="1800" b="0" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1400" b="0" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -2745,7 +2727,7 @@
                                     <m:sSub>
                                       <m:sSubPr>
                                         <m:ctrlPr>
-                                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -2760,7 +2742,7 @@
                                         <m:sSub>
                                           <m:sSubPr>
                                             <m:ctrlPr>
-                                              <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                              <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                                 <a:solidFill>
                                                   <a:schemeClr val="tx1"/>
                                                 </a:solidFill>
@@ -2773,7 +2755,7 @@
                                           </m:sSubPr>
                                           <m:e>
                                             <m:r>
-                                              <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                              <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                                 <a:solidFill>
                                                   <a:schemeClr val="tx1"/>
                                                 </a:solidFill>
@@ -2787,7 +2769,7 @@
                                           </m:e>
                                           <m:sub>
                                             <m:r>
-                                              <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                              <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                                 <a:solidFill>
                                                   <a:schemeClr val="tx1"/>
                                                 </a:solidFill>
@@ -2801,7 +2783,7 @@
                                           </m:sub>
                                         </m:sSub>
                                         <m:r>
-                                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -2815,7 +2797,7 @@
                                       </m:e>
                                       <m:sub>
                                         <m:r>
-                                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -2833,7 +2815,7 @@
                                     <m:sSup>
                                       <m:sSupPr>
                                         <m:ctrlPr>
-                                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -2848,7 +2830,7 @@
                                         <m:d>
                                           <m:dPr>
                                             <m:ctrlPr>
-                                              <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                              <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                                 <a:solidFill>
                                                   <a:schemeClr val="tx1"/>
                                                 </a:solidFill>
@@ -2861,7 +2843,7 @@
                                           </m:dPr>
                                           <m:e>
                                             <m:r>
-                                              <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                              <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                                 <a:solidFill>
                                                   <a:schemeClr val="tx1"/>
                                                 </a:solidFill>
@@ -2873,7 +2855,7 @@
                                               <m:t>1+</m:t>
                                             </m:r>
                                             <m:r>
-                                              <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                                              <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                                                 <a:solidFill>
                                                   <a:schemeClr val="tx1"/>
                                                 </a:solidFill>
@@ -2891,7 +2873,7 @@
                                         <m:func>
                                           <m:funcPr>
                                             <m:ctrlPr>
-                                              <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                                              <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                                                 <a:solidFill>
                                                   <a:schemeClr val="tx1"/>
                                                 </a:solidFill>
@@ -2907,7 +2889,7 @@
                                               <m:rPr>
                                                 <m:sty m:val="p"/>
                                               </m:rPr>
-                                              <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                                              <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                                                 <a:solidFill>
                                                   <a:schemeClr val="tx1"/>
                                                 </a:solidFill>
@@ -2923,7 +2905,7 @@
                                             <m:d>
                                               <m:dPr>
                                                 <m:ctrlPr>
-                                                  <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                                                  <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                                                     <a:solidFill>
                                                       <a:schemeClr val="tx1"/>
                                                     </a:solidFill>
@@ -2936,7 +2918,7 @@
                                               </m:dPr>
                                               <m:e>
                                                 <m:r>
-                                                  <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                                                  <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                                                     <a:solidFill>
                                                       <a:schemeClr val="tx1"/>
                                                     </a:solidFill>
@@ -2948,7 +2930,7 @@
                                                   <m:t>0,</m:t>
                                                 </m:r>
                                                 <m:r>
-                                                  <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                                  <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                                     <a:solidFill>
                                                       <a:schemeClr val="tx1"/>
                                                     </a:solidFill>
@@ -2960,7 +2942,7 @@
                                                   <m:t>𝑖</m:t>
                                                 </m:r>
                                                 <m:r>
-                                                  <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                                                  <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                                                     <a:solidFill>
                                                       <a:schemeClr val="tx1"/>
                                                     </a:solidFill>
@@ -2974,7 +2956,7 @@
                                                 <m:sSub>
                                                   <m:sSubPr>
                                                     <m:ctrlPr>
-                                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                                         <a:solidFill>
                                                           <a:schemeClr val="tx1"/>
                                                         </a:solidFill>
@@ -2987,7 +2969,7 @@
                                                   </m:sSubPr>
                                                   <m:e>
                                                     <m:r>
-                                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                                         <a:solidFill>
                                                           <a:schemeClr val="tx1"/>
                                                         </a:solidFill>
@@ -3001,7 +2983,7 @@
                                                   </m:e>
                                                   <m:sub>
                                                     <m:r>
-                                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                                         <a:solidFill>
                                                           <a:schemeClr val="tx1"/>
                                                         </a:solidFill>
@@ -3027,7 +3009,7 @@
                           </m:e>
                         </m:d>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3039,7 +3021,7 @@
                           <m:t>−</m:t>
                         </m:r>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3055,7 +3037,7 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3068,7 +3050,7 @@
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3082,7 +3064,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3098,7 +3080,7 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3111,7 +3093,7 @@
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3125,7 +3107,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3141,7 +3123,7 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3154,7 +3136,7 @@
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3168,7 +3150,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3184,7 +3166,7 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3197,7 +3179,7 @@
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3211,7 +3193,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3227,7 +3209,7 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3240,7 +3222,7 @@
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3254,7 +3236,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3270,7 +3252,7 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3283,7 +3265,7 @@
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3297,7 +3279,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3311,7 +3293,7 @@
                       </m:sub>
                     </m:sSub>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                      <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                         <a:solidFill>
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
@@ -3323,7 +3305,7 @@
                       <m:t>(1+</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                      <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                         <a:solidFill>
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
@@ -3335,7 +3317,7 @@
                       <m:t>𝐵</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                      <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                         <a:solidFill>
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
@@ -3347,7 +3329,7 @@
                       <m:t>)(1+9</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                      <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                         <a:solidFill>
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
@@ -3359,7 +3341,7 @@
                       <m:t>𝑆</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                      <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                         <a:solidFill>
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
@@ -3373,7 +3355,7 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                          <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -3389,7 +3371,7 @@
                           <m:naryPr>
                             <m:chr m:val="∑"/>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                              <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                 <a:solidFill>
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
@@ -3402,7 +3384,7 @@
                           </m:naryPr>
                           <m:sub>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                              <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                 <a:solidFill>
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
@@ -3414,7 +3396,7 @@
                               <m:t>𝑖</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                              <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                 <a:solidFill>
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
@@ -3428,7 +3410,7 @@
                             <m:sSub>
                               <m:sSubPr>
                                 <m:ctrlPr>
-                                  <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                  <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                     <a:solidFill>
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
@@ -3441,7 +3423,7 @@
                               </m:sSubPr>
                               <m:e>
                                 <m:r>
-                                  <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                  <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                     <a:solidFill>
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
@@ -3455,7 +3437,7 @@
                               </m:e>
                               <m:sub>
                                 <m:r>
-                                  <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                  <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                     <a:solidFill>
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
@@ -3471,7 +3453,7 @@
                           </m:sub>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                              <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                 <a:solidFill>
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
@@ -3487,7 +3469,7 @@
                             <m:f>
                               <m:fPr>
                                 <m:ctrlPr>
-                                  <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                  <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                     <a:solidFill>
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
@@ -3502,7 +3484,7 @@
                                 <m:sSub>
                                   <m:sSubPr>
                                     <m:ctrlPr>
-                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -3515,7 +3497,7 @@
                                   </m:sSubPr>
                                   <m:e>
                                     <m:r>
-                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -3529,7 +3511,7 @@
                                   </m:e>
                                   <m:sub>
                                     <m:r>
-                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -3547,7 +3529,7 @@
                                 <m:sSup>
                                   <m:sSupPr>
                                     <m:ctrlPr>
-                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -3562,7 +3544,7 @@
                                     <m:d>
                                       <m:dPr>
                                         <m:ctrlPr>
-                                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -3575,7 +3557,7 @@
                                       </m:dPr>
                                       <m:e>
                                         <m:r>
-                                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -3587,7 +3569,7 @@
                                           <m:t>1+</m:t>
                                         </m:r>
                                         <m:r>
-                                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -3603,7 +3585,7 @@
                                   </m:e>
                                   <m:sup>
                                     <m:r>
-                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -3615,7 +3597,7 @@
                                       <m:t>𝑖</m:t>
                                     </m:r>
                                     <m:r>
-                                      <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                      <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                         <a:solidFill>
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
@@ -3629,7 +3611,7 @@
                                     <m:sSub>
                                       <m:sSubPr>
                                         <m:ctrlPr>
-                                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -3642,7 +3624,7 @@
                                       </m:sSubPr>
                                       <m:e>
                                         <m:r>
-                                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -3656,7 +3638,7 @@
                                       </m:e>
                                       <m:sub>
                                         <m:r>
-                                          <a:rPr lang="en-US" sz="1600" i="1" kern="1200">
+                                          <a:rPr lang="en-US" sz="1200" i="1" kern="1200">
                                             <a:solidFill>
                                               <a:schemeClr val="tx1"/>
                                             </a:solidFill>
@@ -3678,7 +3660,7 @@
                       </m:e>
                     </m:d>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                      <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                         <a:solidFill>
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
@@ -3690,7 +3672,7 @@
                       <m:t>+</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" i="1" kern="1200">
+                      <a:rPr lang="en-US" sz="1200" b="0" i="1" kern="1200">
                         <a:solidFill>
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
@@ -3704,14 +3686,14 @@
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
-              <a:endParaRPr lang="en-US" sz="2000">
+              <a:endParaRPr lang="en-US" sz="1600">
                 <a:effectLst/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 2">
@@ -3725,8 +3707,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1397000" y="450850"/>
-              <a:ext cx="10464800" cy="1035050"/>
+              <a:off x="8483600" y="7150100"/>
+              <a:ext cx="6781800" cy="787400"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3854,7 +3836,7 @@
             <a:p>
               <a:pPr rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3866,7 +3848,7 @@
                 <a:t>𝑉_𝑃=((∑</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3878,7 +3860,7 @@
                 <a:t>_(𝑖=</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3890,7 +3872,7 @@
                 <a:t>𝑌_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3902,7 +3884,7 @@
                 <a:t>𝑔)^</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3914,7 +3896,7 @@
                 <a:t>2</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3926,31 +3908,31 @@
                 <a:t>0▒(</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1800" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1400" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
                 <a:t>𝑀_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1800" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1400" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
                 <a:t>𝑖</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1800" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1400" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3962,7 +3944,7 @@
                 <a:t>+</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3974,7 +3956,7 @@
                 <a:t>〖</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3986,7 +3968,7 @@
                 <a:t>𝑅_𝑖 𝐿〗_𝑖)/(1+</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3998,7 +3980,7 @@
                 <a:t>𝐼)^max⁡(0,</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4010,7 +3992,7 @@
                 <a:t>𝑖</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4022,7 +4004,7 @@
                 <a:t>−</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4034,7 +4016,7 @@
                 <a:t>𝑌_𝑠 )  )−𝐸) 𝐷_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4046,7 +4028,7 @@
                 <a:t>𝐴 </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4058,7 +4040,7 @@
                 <a:t>𝐷_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4070,7 +4052,7 @@
                 <a:t>𝑈 </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4082,7 +4064,7 @@
                 <a:t>𝐷_𝐹 𝐷_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4094,7 +4076,7 @@
                 <a:t>𝑃 </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4106,7 +4088,7 @@
                 <a:t>𝐷_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4118,7 +4100,7 @@
                 <a:t>𝐸 </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4130,7 +4112,7 @@
                 <a:t>𝐷_</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4142,7 +4124,7 @@
                 <a:t>𝑄 (1+𝐵)(1+9𝑆)−(∑_(</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4154,7 +4136,7 @@
                 <a:t>𝑖=𝑌_𝑠)^20▒𝐶_𝑖/(1+𝐼)^(𝑖−𝑌_𝑠 ) )</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0" kern="1200">
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" kern="1200">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4165,7 +4147,7 @@
                 </a:rPr>
                 <a:t>+𝑍</a:t>
               </a:r>
-              <a:endParaRPr lang="en-US" sz="2000">
+              <a:endParaRPr lang="en-US" sz="1600">
                 <a:effectLst/>
               </a:endParaRPr>
             </a:p>
@@ -4179,13 +4161,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3051175</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4650,15 +4632,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53BF41C8-F90B-409F-99E3-921B17673774}">
-  <dimension ref="B2:O44"/>
+  <dimension ref="B1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.08984375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="4.08984375" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="4.08984375" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="13" customWidth="1"/>
     <col min="4" max="4" width="90.1796875" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.90625" style="11" customWidth="1"/>
     <col min="6" max="6" width="10.1796875" style="11" bestFit="1" customWidth="1"/>
@@ -4669,425 +4651,603 @@
     <col min="16" max="16384" width="8.7265625" style="11"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B1" s="42"/>
+      <c r="C1" s="19"/>
+      <c r="J1" s="19"/>
+    </row>
     <row r="2" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B2" s="50"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>67</v>
+      </c>
       <c r="J2" s="19"/>
     </row>
     <row r="3" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B3" s="50"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="19"/>
       <c r="J3" s="19"/>
     </row>
     <row r="4" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B4" s="50"/>
-      <c r="C4" s="19"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="46" t="s">
+        <v>38</v>
+      </c>
       <c r="J4" s="19"/>
     </row>
     <row r="5" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B5" s="50"/>
-      <c r="C5" s="19"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="56" t="s">
+        <v>43</v>
+      </c>
       <c r="J5" s="19"/>
     </row>
     <row r="6" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B6" s="50"/>
-      <c r="C6" s="19"/>
-      <c r="J6" s="19"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="57" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B7" s="50"/>
-      <c r="C7" s="19"/>
-      <c r="J7" s="19"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="58" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="8" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B8" s="50"/>
-      <c r="C8" s="61" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="19"/>
+    <row r="8" spans="2:15" s="12" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="42"/>
+      <c r="C8" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="9" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B9" s="50"/>
-      <c r="C9" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" s="19"/>
+    <row r="9" spans="2:15" s="12" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="42"/>
+      <c r="C9" s="55">
+        <v>10</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="12">
+        <v>1</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" ref="G9:G28" si="0">IF(F9&lt;$C$14,0,$C$16/MAX(1,($C$10*ABS($C$9-F9))))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="21">
+        <f t="shared" ref="H9:H28" si="1">G9*$C$17</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="21">
+        <f t="shared" ref="I9:I28" si="2">IF(F9&lt;$C$14,0,$C$15/MAX(1,($C$10*ABS($C$9-F9))))</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="22">
+        <f>(H9+I9)/((1+$C$18)^MAX(0,(F9-$C$13)))</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="25">
+        <f>IF(F9&lt;$C$13,"sunk",IF(OR(F9&lt;=$C$14,$C$29="yes"),$C$33,0)+IF(F9=1,$C$32-$C$33,0))</f>
+        <v>12000</v>
+      </c>
+      <c r="M9" s="26">
+        <f>IF(F9&lt;$C$13,"sunk",IF(F9&lt;4,0,500*(1+F9/5)*$C$34*IF($C$29="yes",(1+F9/8),1)))</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="26">
+        <f t="shared" ref="N9:N28" si="3">IF(F9&lt;$C$13,"sunk",L9+M9)</f>
+        <v>12000</v>
+      </c>
+      <c r="O9" s="27">
+        <f t="shared" ref="O9:O28" si="4">IF(N9="sunk",0,N9/(1+$C$18)^MAX(0,(F9-$C$13)))</f>
+        <v>9600</v>
+      </c>
     </row>
-    <row r="10" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B10" s="50"/>
-      <c r="C10" s="59" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" s="12" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B11" s="50"/>
-      <c r="C11" s="60" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.4">
-      <c r="B12" s="50"/>
-      <c r="C12" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="N12" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="50"/>
-      <c r="C13" s="42">
-        <v>10</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="12">
-        <v>1</v>
-      </c>
-      <c r="G13" s="21">
-        <f t="shared" ref="G13:G32" si="0">IF(F13&lt;$C$18,0,$C$20/MAX(1,($C$14*ABS($C$13-F13))))</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="22">
-        <f t="shared" ref="H13:H32" si="1">G13*$C$21</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="22">
-        <f t="shared" ref="I13:I32" si="2">IF(F13&lt;$C$18,0,$C$19/MAX(1,($C$14*ABS($C$13-F13))))</f>
-        <v>0</v>
-      </c>
-      <c r="J13" s="23">
-        <f>(H13+I13)/((1+$C$22)^MAX(0,(F13-$C$17)))</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="26">
-        <f>IF(F13&lt;$C$17,"sunk",IF(OR(F13&lt;=$C$18,$C$33="yes"),$C$37,0)+IF(F13=1,$C$36-$C$37,0))</f>
-        <v>12000</v>
-      </c>
-      <c r="M13" s="27">
-        <f>IF(F13&lt;$C$17,"sunk",IF(F13&lt;4,0,500*(1+F13/5)*$C$38*IF($C$33="yes",(1+F13/8),1)))</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="27">
-        <f t="shared" ref="N13:N32" si="3">IF(F13&lt;$C$17,"sunk",L13+M13)</f>
-        <v>12000</v>
-      </c>
-      <c r="O13" s="28">
-        <f t="shared" ref="O13:O32" si="4">IF(N13="sunk",0,N13/(1+$C$22)^MAX(0,(F13-$C$17)))</f>
-        <v>9600</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="52"/>
-      <c r="C14" s="42">
+    <row r="10" spans="2:15" s="10" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="44"/>
+      <c r="C10" s="55">
         <v>0.4</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="12">
-        <f>F13+1</f>
+      <c r="F10" s="12">
+        <f>F9+1</f>
         <v>2</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G10" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H10" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="24">
+        <f t="shared" ref="J10:J28" si="5">(H10+I10)/((1+$C$18)^MAX(0,(F10-$C$13)))</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="28">
+        <f t="shared" ref="L10:L28" si="6">IF(F10&lt;$C$13,"sunk",IF(OR(F10&lt;=$C$14,$C$29="yes"),$C$33,0)+IF(F10=1,$C$32-$C$33,0))</f>
+        <v>8000</v>
+      </c>
+      <c r="M10" s="18">
+        <f t="shared" ref="M10:M28" si="7">IF(F10&lt;$C$13,"sunk",IF(F10&lt;4,0,500*(1+F10/5)*$C$34*IF($C$29="yes",(1+F10/8),1)))</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="18">
+        <f t="shared" si="3"/>
+        <v>8000</v>
+      </c>
+      <c r="O10" s="29">
+        <f t="shared" si="4"/>
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="19"/>
+      <c r="D11" s="12"/>
+      <c r="F11" s="12">
+        <f t="shared" ref="F11:F28" si="8">F10+1</f>
+        <v>3</v>
+      </c>
+      <c r="G11" s="23">
+        <f t="shared" si="0"/>
+        <v>2857142.8571428568</v>
+      </c>
+      <c r="H11" s="17">
+        <f t="shared" si="1"/>
+        <v>428571.42857142852</v>
+      </c>
+      <c r="I11" s="17">
+        <f t="shared" si="2"/>
+        <v>714285.7142857142</v>
+      </c>
+      <c r="J11" s="24">
+        <f t="shared" si="5"/>
+        <v>585142.85714285704</v>
+      </c>
+      <c r="L11" s="28">
+        <f t="shared" si="6"/>
+        <v>8000</v>
+      </c>
+      <c r="M11" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="18">
+        <f t="shared" si="3"/>
+        <v>8000</v>
+      </c>
+      <c r="O11" s="29">
+        <f t="shared" si="4"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="42"/>
+      <c r="C12" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="0"/>
+        <v>3333333.333333333</v>
+      </c>
+      <c r="H12" s="17">
+        <f t="shared" si="1"/>
+        <v>499999.99999999994</v>
+      </c>
+      <c r="I12" s="17">
+        <f t="shared" si="2"/>
+        <v>833333.33333333326</v>
+      </c>
+      <c r="J12" s="24">
+        <f t="shared" si="5"/>
+        <v>546133.33333333326</v>
+      </c>
+      <c r="L12" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="18">
+        <f t="shared" si="7"/>
+        <v>900</v>
+      </c>
+      <c r="N12" s="18">
+        <f t="shared" si="3"/>
+        <v>900</v>
+      </c>
+      <c r="O12" s="29">
+        <f t="shared" si="4"/>
+        <v>368.64</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="51">
+        <v>0</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="0"/>
+        <v>4000000</v>
+      </c>
+      <c r="H13" s="17">
+        <f t="shared" si="1"/>
+        <v>600000</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" si="2"/>
+        <v>1000000</v>
+      </c>
+      <c r="J13" s="24">
+        <f t="shared" si="5"/>
+        <v>524288</v>
+      </c>
+      <c r="L13" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="18">
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="N13" s="18">
+        <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="O13" s="29">
+        <f t="shared" si="4"/>
+        <v>327.68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="51">
+        <v>3</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="0"/>
+        <v>5000000</v>
+      </c>
       <c r="H14" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>750000</v>
       </c>
       <c r="I14" s="17">
         <f t="shared" si="2"/>
+        <v>1250000</v>
+      </c>
+      <c r="J14" s="24">
+        <f t="shared" si="5"/>
+        <v>524288</v>
+      </c>
+      <c r="L14" s="28">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J14" s="25">
-        <f t="shared" ref="J14:J32" si="5">(H14+I14)/((1+$C$22)^MAX(0,(F14-$C$17)))</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="29">
-        <f t="shared" ref="L14:L32" si="6">IF(F14&lt;$C$17,"sunk",IF(OR(F14&lt;=$C$18,$C$33="yes"),$C$37,0)+IF(F14=1,$C$36-$C$37,0))</f>
-        <v>8000</v>
-      </c>
       <c r="M14" s="18">
-        <f t="shared" ref="M14:M32" si="7">IF(F14&lt;$C$17,"sunk",IF(F14&lt;4,0,500*(1+F14/5)*$C$38*IF($C$33="yes",(1+F14/8),1)))</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1100</v>
       </c>
       <c r="N14" s="18">
         <f t="shared" si="3"/>
-        <v>8000</v>
-      </c>
-      <c r="O14" s="30">
+        <v>1100</v>
+      </c>
+      <c r="O14" s="29">
         <f t="shared" si="4"/>
-        <v>5120</v>
+        <v>288.35840000000002</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="C15" s="19"/>
-      <c r="D15" s="12"/>
+    <row r="15" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="48">
+        <v>2000000</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="F15" s="12">
-        <f t="shared" ref="F15:F32" si="8">F14+1</f>
-        <v>3</v>
-      </c>
-      <c r="G15" s="24">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="G15" s="23">
         <f t="shared" si="0"/>
-        <v>2857142.8571428568</v>
+        <v>6666666.666666666</v>
       </c>
       <c r="H15" s="17">
         <f t="shared" si="1"/>
-        <v>428571.42857142852</v>
+        <v>999999.99999999988</v>
       </c>
       <c r="I15" s="17">
         <f t="shared" si="2"/>
-        <v>714285.7142857142</v>
-      </c>
-      <c r="J15" s="25">
+        <v>1666666.6666666665</v>
+      </c>
+      <c r="J15" s="24">
         <f t="shared" si="5"/>
-        <v>585142.85714285704</v>
-      </c>
-      <c r="L15" s="29">
+        <v>559240.53333333333</v>
+      </c>
+      <c r="L15" s="28">
         <f t="shared" si="6"/>
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="M15" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="N15" s="18">
         <f t="shared" si="3"/>
-        <v>8000</v>
-      </c>
-      <c r="O15" s="30">
+        <v>1200</v>
+      </c>
+      <c r="O15" s="29">
         <f t="shared" si="4"/>
-        <v>4096</v>
+        <v>251.65824000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B16" s="50"/>
-      <c r="C16" s="50" t="s">
-        <v>37</v>
+    <row r="16" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="48">
+        <v>8000000</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="F16" s="12">
         <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="G16" s="24">
+        <v>8</v>
+      </c>
+      <c r="G16" s="23">
         <f t="shared" si="0"/>
-        <v>3333333.333333333</v>
+        <v>8000000</v>
       </c>
       <c r="H16" s="17">
         <f t="shared" si="1"/>
-        <v>499999.99999999994</v>
+        <v>1200000</v>
       </c>
       <c r="I16" s="17">
         <f t="shared" si="2"/>
-        <v>833333.33333333326</v>
-      </c>
-      <c r="J16" s="25">
+        <v>2000000</v>
+      </c>
+      <c r="J16" s="24">
         <f t="shared" si="5"/>
-        <v>546133.33333333326</v>
-      </c>
-      <c r="L16" s="29">
+        <v>536870.91200000001</v>
+      </c>
+      <c r="L16" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M16" s="18">
         <f t="shared" si="7"/>
-        <v>900</v>
+        <v>1300</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" si="3"/>
-        <v>900</v>
-      </c>
-      <c r="O16" s="30">
+        <v>1300</v>
+      </c>
+      <c r="O16" s="29">
         <f t="shared" si="4"/>
-        <v>368.64</v>
+        <v>218.10380799999999</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="16" x14ac:dyDescent="0.4">
-      <c r="B17" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="45">
-        <v>0</v>
+    <row r="17" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="52">
+        <v>0.15</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F17" s="12">
         <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="G17" s="24">
+        <v>9</v>
+      </c>
+      <c r="G17" s="23">
         <f t="shared" si="0"/>
-        <v>4000000</v>
+        <v>8000000</v>
       </c>
       <c r="H17" s="17">
         <f t="shared" si="1"/>
-        <v>600000</v>
+        <v>1200000</v>
       </c>
       <c r="I17" s="17">
         <f t="shared" si="2"/>
-        <v>1000000</v>
-      </c>
-      <c r="J17" s="25">
+        <v>2000000</v>
+      </c>
+      <c r="J17" s="24">
         <f t="shared" si="5"/>
-        <v>524288</v>
-      </c>
-      <c r="L17" s="29">
+        <v>429496.72960000002</v>
+      </c>
+      <c r="L17" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M17" s="18">
         <f t="shared" si="7"/>
-        <v>1000</v>
+        <v>1400</v>
       </c>
       <c r="N17" s="18">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="O17" s="30">
+        <v>1400</v>
+      </c>
+      <c r="O17" s="29">
         <f t="shared" si="4"/>
-        <v>327.68</v>
+        <v>187.90481919999999</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="16" x14ac:dyDescent="0.4">
-      <c r="B18" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="45">
-        <v>3</v>
+    <row r="18" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="52">
+        <v>0.25</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="G18" s="24">
+        <v>10</v>
+      </c>
+      <c r="G18" s="23">
         <f t="shared" si="0"/>
-        <v>5000000</v>
+        <v>8000000</v>
       </c>
       <c r="H18" s="17">
         <f t="shared" si="1"/>
-        <v>750000</v>
+        <v>1200000</v>
       </c>
       <c r="I18" s="17">
         <f t="shared" si="2"/>
-        <v>1250000</v>
-      </c>
-      <c r="J18" s="25">
+        <v>2000000</v>
+      </c>
+      <c r="J18" s="24">
         <f t="shared" si="5"/>
-        <v>524288</v>
-      </c>
-      <c r="L18" s="29">
+        <v>343597.38368000003</v>
+      </c>
+      <c r="L18" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M18" s="18">
         <f t="shared" si="7"/>
-        <v>1100</v>
+        <v>1500</v>
       </c>
       <c r="N18" s="18">
         <f t="shared" si="3"/>
-        <v>1100</v>
-      </c>
-      <c r="O18" s="30">
+        <v>1500</v>
+      </c>
+      <c r="O18" s="29">
         <f t="shared" si="4"/>
-        <v>288.35840000000002</v>
+        <v>161.06127359999999</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B19" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="56">
+    <row r="19" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="49">
         <v>2000000</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F19" s="12">
         <f t="shared" si="8"/>
-        <v>7</v>
-      </c>
-      <c r="G19" s="24">
+        <v>11</v>
+      </c>
+      <c r="G19" s="23">
         <f t="shared" si="0"/>
-        <v>6666666.666666666</v>
+        <v>8000000</v>
       </c>
       <c r="H19" s="17">
         <f t="shared" si="1"/>
-        <v>999999.99999999988</v>
+        <v>1200000</v>
       </c>
       <c r="I19" s="17">
         <f t="shared" si="2"/>
-        <v>1666666.6666666665</v>
-      </c>
-      <c r="J19" s="25">
+        <v>2000000</v>
+      </c>
+      <c r="J19" s="24">
         <f t="shared" si="5"/>
-        <v>559240.53333333333</v>
-      </c>
-      <c r="L19" s="29">
+        <v>274877.90694399999</v>
+      </c>
+      <c r="L19" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M19" s="18">
         <f t="shared" si="7"/>
-        <v>1200</v>
+        <v>1600</v>
       </c>
       <c r="N19" s="18">
         <f t="shared" si="3"/>
-        <v>1200</v>
-      </c>
-      <c r="O19" s="30">
+        <v>1600</v>
+      </c>
+      <c r="O19" s="29">
         <f t="shared" si="4"/>
-        <v>251.65824000000001</v>
+        <v>137.43895347200001</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B20" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="56">
-        <v>8000000</v>
+    <row r="20" spans="2:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="52">
+        <v>0.5</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F20" s="12">
         <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="G20" s="24">
+        <v>12</v>
+      </c>
+      <c r="G20" s="23">
         <f t="shared" si="0"/>
         <v>8000000</v>
       </c>
@@ -5099,816 +5259,624 @@
         <f t="shared" si="2"/>
         <v>2000000</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="24">
         <f t="shared" si="5"/>
-        <v>536870.91200000001</v>
-      </c>
-      <c r="L20" s="29">
+        <v>219902.32555519999</v>
+      </c>
+      <c r="L20" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M20" s="18">
         <f t="shared" si="7"/>
-        <v>1300</v>
+        <v>1700</v>
       </c>
       <c r="N20" s="18">
         <f t="shared" si="3"/>
-        <v>1300</v>
-      </c>
-      <c r="O20" s="30">
+        <v>1700</v>
+      </c>
+      <c r="O20" s="29">
         <f t="shared" si="4"/>
-        <v>218.10380799999999</v>
+        <v>116.82311045119999</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B21" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="46">
-        <v>0.15</v>
+    <row r="21" spans="2:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="53">
+        <v>0.5</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F21" s="12">
         <f t="shared" si="8"/>
-        <v>9</v>
-      </c>
-      <c r="G21" s="24">
+        <v>13</v>
+      </c>
+      <c r="G21" s="23">
         <f t="shared" si="0"/>
-        <v>8000000</v>
+        <v>6666666.666666666</v>
       </c>
       <c r="H21" s="17">
         <f t="shared" si="1"/>
-        <v>1200000</v>
+        <v>999999.99999999988</v>
       </c>
       <c r="I21" s="17">
         <f t="shared" si="2"/>
-        <v>2000000</v>
-      </c>
-      <c r="J21" s="25">
+        <v>1666666.6666666665</v>
+      </c>
+      <c r="J21" s="24">
         <f t="shared" si="5"/>
-        <v>429496.72960000002</v>
-      </c>
-      <c r="L21" s="29">
+        <v>146601.55037013334</v>
+      </c>
+      <c r="L21" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M21" s="18">
         <f t="shared" si="7"/>
-        <v>1400</v>
+        <v>1800</v>
       </c>
       <c r="N21" s="18">
         <f t="shared" si="3"/>
-        <v>1400</v>
-      </c>
-      <c r="O21" s="30">
+        <v>1800</v>
+      </c>
+      <c r="O21" s="29">
         <f t="shared" si="4"/>
-        <v>187.90481919999999</v>
+        <v>98.956046499839999</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B22" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="46">
-        <v>0.25</v>
+    <row r="22" spans="2:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="53">
+        <v>1</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F22" s="12">
         <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="G22" s="24">
+        <v>14</v>
+      </c>
+      <c r="G22" s="23">
         <f t="shared" si="0"/>
-        <v>8000000</v>
+        <v>5000000</v>
       </c>
       <c r="H22" s="17">
         <f t="shared" si="1"/>
-        <v>1200000</v>
+        <v>750000</v>
       </c>
       <c r="I22" s="17">
         <f t="shared" si="2"/>
-        <v>2000000</v>
-      </c>
-      <c r="J22" s="25">
+        <v>1250000</v>
+      </c>
+      <c r="J22" s="24">
         <f t="shared" si="5"/>
-        <v>343597.38368000003</v>
-      </c>
-      <c r="L22" s="29">
+        <v>87960.930222080002</v>
+      </c>
+      <c r="L22" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M22" s="18">
         <f t="shared" si="7"/>
-        <v>1500</v>
+        <v>1900</v>
       </c>
       <c r="N22" s="18">
         <f t="shared" si="3"/>
-        <v>1500</v>
-      </c>
-      <c r="O22" s="30">
+        <v>1900</v>
+      </c>
+      <c r="O22" s="29">
         <f t="shared" si="4"/>
-        <v>161.06127359999999</v>
+        <v>83.562883710975996</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B23" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="57">
-        <v>2000000</v>
+    <row r="23" spans="2:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="53">
+        <v>0.4</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" si="8"/>
-        <v>11</v>
-      </c>
-      <c r="G23" s="24">
+        <v>15</v>
+      </c>
+      <c r="G23" s="23">
         <f t="shared" si="0"/>
-        <v>8000000</v>
+        <v>4000000</v>
       </c>
       <c r="H23" s="17">
         <f t="shared" si="1"/>
-        <v>1200000</v>
+        <v>600000</v>
       </c>
       <c r="I23" s="17">
         <f t="shared" si="2"/>
-        <v>2000000</v>
-      </c>
-      <c r="J23" s="25">
+        <v>1000000</v>
+      </c>
+      <c r="J23" s="24">
         <f t="shared" si="5"/>
-        <v>274877.90694399999</v>
-      </c>
-      <c r="L23" s="29">
+        <v>56294.995342131202</v>
+      </c>
+      <c r="L23" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M23" s="18">
         <f t="shared" si="7"/>
-        <v>1600</v>
+        <v>2000</v>
       </c>
       <c r="N23" s="18">
         <f t="shared" si="3"/>
-        <v>1600</v>
-      </c>
-      <c r="O23" s="30">
+        <v>2000</v>
+      </c>
+      <c r="O23" s="29">
         <f t="shared" si="4"/>
-        <v>137.43895347200001</v>
+        <v>70.368744177663999</v>
       </c>
     </row>
-    <row r="24" spans="2:15" ht="16" x14ac:dyDescent="0.4">
-      <c r="B24" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="46">
-        <v>0.5</v>
+    <row r="24" spans="2:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="54">
+        <v>0.9</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="G24" s="24">
+        <v>16</v>
+      </c>
+      <c r="G24" s="23">
         <f t="shared" si="0"/>
-        <v>8000000</v>
+        <v>3333333.333333333</v>
       </c>
       <c r="H24" s="17">
         <f t="shared" si="1"/>
-        <v>1200000</v>
+        <v>499999.99999999994</v>
       </c>
       <c r="I24" s="17">
         <f t="shared" si="2"/>
-        <v>2000000</v>
-      </c>
-      <c r="J24" s="25">
+        <v>833333.33333333326</v>
+      </c>
+      <c r="J24" s="24">
         <f t="shared" si="5"/>
-        <v>219902.32555519999</v>
-      </c>
-      <c r="L24" s="29">
+        <v>37529.996894754135</v>
+      </c>
+      <c r="L24" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M24" s="18">
         <f t="shared" si="7"/>
-        <v>1700</v>
+        <v>2100</v>
       </c>
       <c r="N24" s="18">
         <f t="shared" si="3"/>
-        <v>1700</v>
-      </c>
-      <c r="O24" s="30">
+        <v>2100</v>
+      </c>
+      <c r="O24" s="29">
         <f t="shared" si="4"/>
-        <v>116.82311045119999</v>
+        <v>59.109745109237757</v>
       </c>
     </row>
-    <row r="25" spans="2:15" ht="16" x14ac:dyDescent="0.4">
-      <c r="B25" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="47">
-        <v>0.5</v>
+    <row r="25" spans="2:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="54">
+        <v>0.8</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="8"/>
-        <v>13</v>
-      </c>
-      <c r="G25" s="24">
+        <v>17</v>
+      </c>
+      <c r="G25" s="23">
         <f t="shared" si="0"/>
-        <v>6666666.666666666</v>
+        <v>2857142.8571428568</v>
       </c>
       <c r="H25" s="17">
         <f t="shared" si="1"/>
-        <v>999999.99999999988</v>
+        <v>428571.42857142852</v>
       </c>
       <c r="I25" s="17">
         <f t="shared" si="2"/>
-        <v>1666666.6666666665</v>
-      </c>
-      <c r="J25" s="25">
+        <v>714285.7142857142</v>
+      </c>
+      <c r="J25" s="24">
         <f t="shared" si="5"/>
-        <v>146601.55037013334</v>
-      </c>
-      <c r="L25" s="29">
+        <v>25734.85501354569</v>
+      </c>
+      <c r="L25" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M25" s="18">
         <f t="shared" si="7"/>
-        <v>1800</v>
+        <v>2200</v>
       </c>
       <c r="N25" s="18">
         <f t="shared" si="3"/>
-        <v>1800</v>
-      </c>
-      <c r="O25" s="30">
+        <v>2200</v>
+      </c>
+      <c r="O25" s="29">
         <f t="shared" si="4"/>
-        <v>98.956046499839999</v>
+        <v>49.539595901075458</v>
       </c>
     </row>
-    <row r="26" spans="2:15" ht="16" x14ac:dyDescent="0.4">
-      <c r="B26" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="47">
-        <v>1</v>
+    <row r="26" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="52">
+        <v>0.25</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F26" s="12">
         <f t="shared" si="8"/>
-        <v>14</v>
-      </c>
-      <c r="G26" s="24">
+        <v>18</v>
+      </c>
+      <c r="G26" s="23">
         <f t="shared" si="0"/>
-        <v>5000000</v>
+        <v>2500000</v>
       </c>
       <c r="H26" s="17">
         <f t="shared" si="1"/>
-        <v>750000</v>
+        <v>375000</v>
       </c>
       <c r="I26" s="17">
         <f t="shared" si="2"/>
-        <v>1250000</v>
-      </c>
-      <c r="J26" s="25">
+        <v>625000</v>
+      </c>
+      <c r="J26" s="24">
         <f t="shared" si="5"/>
-        <v>87960.930222080002</v>
-      </c>
-      <c r="L26" s="29">
+        <v>18014.398509481984</v>
+      </c>
+      <c r="L26" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M26" s="18">
         <f t="shared" si="7"/>
-        <v>1900</v>
+        <v>2300</v>
       </c>
       <c r="N26" s="18">
         <f t="shared" si="3"/>
-        <v>1900</v>
-      </c>
-      <c r="O26" s="30">
+        <v>2300</v>
+      </c>
+      <c r="O26" s="29">
         <f t="shared" si="4"/>
-        <v>83.562883710975996</v>
+        <v>41.433116571808561</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="16" x14ac:dyDescent="0.4">
-      <c r="B27" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="47">
-        <v>0.4</v>
+    <row r="27" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="53">
+        <v>0</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="8"/>
-        <v>15</v>
-      </c>
-      <c r="G27" s="24">
+        <v>19</v>
+      </c>
+      <c r="G27" s="23">
         <f t="shared" si="0"/>
-        <v>4000000</v>
+        <v>2222222.222222222</v>
       </c>
       <c r="H27" s="17">
         <f t="shared" si="1"/>
-        <v>600000</v>
+        <v>333333.33333333331</v>
       </c>
       <c r="I27" s="17">
         <f t="shared" si="2"/>
-        <v>1000000</v>
-      </c>
-      <c r="J27" s="25">
+        <v>555555.5555555555</v>
+      </c>
+      <c r="J27" s="24">
         <f t="shared" si="5"/>
-        <v>56294.995342131202</v>
-      </c>
-      <c r="L27" s="29">
+        <v>12810.238940076075</v>
+      </c>
+      <c r="L27" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M27" s="18">
         <f t="shared" si="7"/>
-        <v>2000</v>
+        <v>2400</v>
       </c>
       <c r="N27" s="18">
         <f t="shared" si="3"/>
-        <v>2000</v>
-      </c>
-      <c r="O27" s="30">
+        <v>2400</v>
+      </c>
+      <c r="O27" s="29">
         <f t="shared" si="4"/>
-        <v>70.368744177663999</v>
+        <v>34.58764513820541</v>
       </c>
     </row>
-    <row r="28" spans="2:15" ht="16" x14ac:dyDescent="0.4">
-      <c r="B28" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="48">
-        <v>0.9</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>54</v>
-      </c>
+    <row r="28" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C28" s="47"/>
       <c r="F28" s="12">
         <f t="shared" si="8"/>
-        <v>16</v>
-      </c>
-      <c r="G28" s="24">
+        <v>20</v>
+      </c>
+      <c r="G28" s="23">
         <f t="shared" si="0"/>
-        <v>3333333.333333333</v>
+        <v>2000000</v>
       </c>
       <c r="H28" s="17">
         <f t="shared" si="1"/>
-        <v>499999.99999999994</v>
+        <v>300000</v>
       </c>
       <c r="I28" s="17">
         <f t="shared" si="2"/>
-        <v>833333.33333333326</v>
-      </c>
-      <c r="J28" s="25">
+        <v>500000</v>
+      </c>
+      <c r="J28" s="24">
         <f t="shared" si="5"/>
-        <v>37529.996894754135</v>
-      </c>
-      <c r="L28" s="29">
+        <v>9223.3720368547765</v>
+      </c>
+      <c r="L28" s="38">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M28" s="18">
-        <f t="shared" si="7"/>
-        <v>2100</v>
-      </c>
-      <c r="N28" s="18">
-        <f t="shared" si="3"/>
-        <v>2100</v>
-      </c>
-      <c r="O28" s="30">
-        <f t="shared" si="4"/>
-        <v>59.109745109237757</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" ht="16" x14ac:dyDescent="0.4">
-      <c r="B29" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="48">
-        <v>0.8</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="12">
-        <f t="shared" si="8"/>
-        <v>17</v>
-      </c>
-      <c r="G29" s="24">
-        <f t="shared" si="0"/>
-        <v>2857142.8571428568</v>
-      </c>
-      <c r="H29" s="17">
-        <f t="shared" si="1"/>
-        <v>428571.42857142852</v>
-      </c>
-      <c r="I29" s="17">
-        <f t="shared" si="2"/>
-        <v>714285.7142857142</v>
-      </c>
-      <c r="J29" s="25">
-        <f t="shared" si="5"/>
-        <v>25734.85501354569</v>
-      </c>
-      <c r="L29" s="29">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="18">
-        <f t="shared" si="7"/>
-        <v>2200</v>
-      </c>
-      <c r="N29" s="18">
-        <f t="shared" si="3"/>
-        <v>2200</v>
-      </c>
-      <c r="O29" s="30">
-        <f t="shared" si="4"/>
-        <v>49.539595901075458</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B30" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="46">
-        <v>0.25</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30" s="12">
-        <f t="shared" si="8"/>
-        <v>18</v>
-      </c>
-      <c r="G30" s="24">
-        <f t="shared" si="0"/>
-        <v>2500000</v>
-      </c>
-      <c r="H30" s="17">
-        <f t="shared" si="1"/>
-        <v>375000</v>
-      </c>
-      <c r="I30" s="17">
-        <f t="shared" si="2"/>
-        <v>625000</v>
-      </c>
-      <c r="J30" s="25">
-        <f t="shared" si="5"/>
-        <v>18014.398509481984</v>
-      </c>
-      <c r="L30" s="29">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="18">
-        <f t="shared" si="7"/>
-        <v>2300</v>
-      </c>
-      <c r="N30" s="18">
-        <f t="shared" si="3"/>
-        <v>2300</v>
-      </c>
-      <c r="O30" s="30">
-        <f t="shared" si="4"/>
-        <v>41.433116571808561</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B31" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="47">
-        <v>0</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F31" s="12">
-        <f t="shared" si="8"/>
-        <v>19</v>
-      </c>
-      <c r="G31" s="24">
-        <f t="shared" si="0"/>
-        <v>2222222.222222222</v>
-      </c>
-      <c r="H31" s="17">
-        <f t="shared" si="1"/>
-        <v>333333.33333333331</v>
-      </c>
-      <c r="I31" s="17">
-        <f t="shared" si="2"/>
-        <v>555555.5555555555</v>
-      </c>
-      <c r="J31" s="25">
-        <f t="shared" si="5"/>
-        <v>12810.238940076075</v>
-      </c>
-      <c r="L31" s="29">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="18">
-        <f t="shared" si="7"/>
-        <v>2400</v>
-      </c>
-      <c r="N31" s="18">
-        <f t="shared" si="3"/>
-        <v>2400</v>
-      </c>
-      <c r="O31" s="30">
-        <f t="shared" si="4"/>
-        <v>34.58764513820541</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="C32" s="49"/>
-      <c r="F32" s="12">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="G32" s="24">
-        <f t="shared" si="0"/>
-        <v>2000000</v>
-      </c>
-      <c r="H32" s="17">
-        <f t="shared" si="1"/>
-        <v>300000</v>
-      </c>
-      <c r="I32" s="17">
-        <f t="shared" si="2"/>
-        <v>500000</v>
-      </c>
-      <c r="J32" s="25">
-        <f t="shared" si="5"/>
-        <v>9223.3720368547765</v>
-      </c>
-      <c r="L32" s="39">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="40">
+      <c r="M28" s="39">
         <f t="shared" si="7"/>
         <v>2500</v>
       </c>
-      <c r="N32" s="40">
+      <c r="N28" s="39">
         <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="O32" s="41">
+      <c r="O28" s="40">
         <f t="shared" si="4"/>
         <v>28.823037615171174</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="C33" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="12" t="s">
+    <row r="29" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C29" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="19" t="s">
+      <c r="E29" s="12"/>
+      <c r="F29" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="33">
-        <f t="shared" ref="G33:J33" si="9">SUM(G13:G32)</f>
+      <c r="G29" s="32">
+        <f t="shared" ref="G29:J29" si="9">SUM(G9:G28)</f>
         <v>90436507.936507925</v>
       </c>
-      <c r="H33" s="34">
+      <c r="H29" s="33">
         <f t="shared" si="9"/>
         <v>13565476.190476192</v>
       </c>
-      <c r="I33" s="34">
+      <c r="I29" s="33">
         <f t="shared" si="9"/>
         <v>22609126.984126981</v>
       </c>
-      <c r="J33" s="35">
+      <c r="J29" s="34">
         <f t="shared" si="9"/>
         <v>4938008.3189177802</v>
       </c>
-      <c r="L33" s="36">
-        <f>SUM(L13:L32)</f>
+      <c r="L29" s="35">
+        <f>SUM(L9:L28)</f>
         <v>28000</v>
       </c>
-      <c r="M33" s="37">
-        <f>SUM(M13:M32)</f>
+      <c r="M29" s="36">
+        <f>SUM(M9:M28)</f>
         <v>28900</v>
       </c>
-      <c r="N33" s="37">
-        <f>SUM(N13:N32)</f>
+      <c r="N29" s="36">
+        <f>SUM(N9:N28)</f>
         <v>56900</v>
       </c>
-      <c r="O33" s="38">
-        <f>SUM(O13:O32)</f>
+      <c r="O29" s="37">
+        <f>SUM(O9:O28)</f>
         <v>21340.049419447179</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="C34" s="19"/>
+    <row r="30" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="19"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" s="31">
+        <f>($J$29-$C$19)*$C$20*$C$21*$C$22*$C$23*$C$24*$C$25*IF(C29="yes",(1+$C$26),1)*(1+9*$C$27)</f>
+        <v>211536.5989620802</v>
+      </c>
+      <c r="M30" s="12"/>
+      <c r="N30" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="O30" s="30">
+        <f>O29</f>
+        <v>21340.049419447179</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+    </row>
+    <row r="32" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="42"/>
+      <c r="C32" s="49">
+        <v>12000</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+    </row>
+    <row r="33" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="42"/>
+      <c r="C33" s="49">
+        <v>8000</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="42"/>
+      <c r="C34" s="50">
+        <v>1</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="32">
-        <f>($J$33-$C$23)*$C$24*$C$25*$C$26*$C$27*$C$28*$C$29*IF(C33="yes",(1+$C$30),1)*(1+9*$C$31)</f>
-        <v>211536.5989620802</v>
-      </c>
-      <c r="M34" s="12"/>
-      <c r="N34" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="O34" s="31">
-        <f>O33</f>
-        <v>21340.049419447179</v>
-      </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B35" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>64</v>
-      </c>
+    <row r="35" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C35" s="47"/>
       <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B36" s="50"/>
-      <c r="C36" s="57">
-        <v>12000</v>
+    <row r="36" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="48">
+        <v>10000</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
+        <v>49</v>
+      </c>
+      <c r="J36" s="11"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B37" s="50"/>
-      <c r="C37" s="57">
-        <v>8000</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+    <row r="37" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="11"/>
+      <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B38" s="50"/>
-      <c r="C38" s="43">
-        <v>1</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="12"/>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J38" s="11"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="C39" s="49"/>
-      <c r="E39" s="12"/>
+    <row r="39" spans="2:10" ht="18" x14ac:dyDescent="0.4">
+      <c r="B39" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="60">
+        <f>J30-O30+$C$36*($C$34)</f>
+        <v>200196.54954263303</v>
+      </c>
+      <c r="D39" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="J39" s="11"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B40" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="56">
-        <v>10000</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="J40" s="11"/>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B41" s="11"/>
-      <c r="J41" s="11"/>
-    </row>
-    <row r="42" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J42" s="11"/>
-    </row>
-    <row r="43" spans="2:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="55">
-        <f>J34-O34+$C$40*($C$38)</f>
-        <v>200196.54954263303</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E43" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="J43" s="11"/>
-    </row>
-    <row r="44" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <conditionalFormatting sqref="C20 C24:C29">
+  <conditionalFormatting sqref="C16 C20:C25">
     <cfRule type="cellIs" dxfId="12" priority="31" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="C17">
     <cfRule type="cellIs" dxfId="11" priority="30" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
+  <conditionalFormatting sqref="C18">
     <cfRule type="cellIs" dxfId="10" priority="27" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O34">
+  <conditionalFormatting sqref="O30">
     <cfRule type="cellIs" dxfId="9" priority="22" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
+  <conditionalFormatting sqref="C39">
     <cfRule type="cellIs" dxfId="8" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34">
+  <conditionalFormatting sqref="J30">
     <cfRule type="cellIs" dxfId="7" priority="15" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C33">
     <cfRule type="cellIs" dxfId="6" priority="12" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
+  <conditionalFormatting sqref="C19">
     <cfRule type="cellIs" dxfId="5" priority="9" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="C36">
     <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
+  <conditionalFormatting sqref="C34">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
+  <conditionalFormatting sqref="C29">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
+  <conditionalFormatting sqref="C7">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
+  <conditionalFormatting sqref="C26">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33" xr:uid="{27368C8D-F909-4D3A-95A3-202A96031B32}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29" xr:uid="{27368C8D-F909-4D3A-95A3-202A96031B32}">
       <formula1>"no,yes"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>